<commit_message>
now it could be no criteria in the table
</commit_message>
<xml_diff>
--- a/src/test/testResources/out.xlsx
+++ b/src/test/testResources/out.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>a</t>
+    <t>HelloOne WorldПривет twoмир!</t>
   </si>
 </sst>
 </file>
@@ -66,17 +66,17 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" t="n">
+        <v>49.0</v>
       </c>
       <c r="B1" t="n">
-        <v>0.0</v>
+        <v>-5.0</v>
       </c>
       <c r="C1" t="n">
-        <v>0.0</v>
+        <v>1.0E38</v>
       </c>
-      <c r="D1" t="n">
-        <v>0.0</v>
+      <c r="D1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>